<commit_message>
baselines MASS UPDATE Repair and REUSE
Changed Repowering to REUSE throughout
Added Merchant Tail
Changed mod_Repairing to mod_Repair
</commit_message>
<xml_diff>
--- a/tests/sensitivity_test.xlsx
+++ b/tests/sensitivity_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sayala\Documents\GitHub\CircularEconomy-MassFlowCalculator\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D28DF2-A8AC-416A-88D4-E18C752B066E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2601AE-42C6-4A39-8695-90BDFDEE4775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{579D3F75-4888-4229-BB5D-2EA286198119}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{579D3F75-4888-4229-BB5D-2EA286198119}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,12 +108,6 @@
     <t>mod_EOL_collected_recycled</t>
   </si>
   <si>
-    <t>mod_Repowering</t>
-  </si>
-  <si>
-    <t>mod_Repairing</t>
-  </si>
-  <si>
     <t>EOL_CE_Pathways</t>
   </si>
   <si>
@@ -138,15 +132,9 @@
     <t>mod_reliability_t50, mod_reliability_t90, mod_lifetime</t>
   </si>
   <si>
-    <t>mod_EOL_collection_eff, mod_EOL_collected_recycled, mod_Repowering, mod_Repairing</t>
-  </si>
-  <si>
     <t>mat_MFG_scrap_Recycled, mat_MFG_scrap_Recycling_eff, mat_MFG_scrap_Recycled_into_HQ, mat_MFG_scrap_Recycled_into_HQ_Reused4MFG</t>
   </si>
   <si>
-    <t>mod_EOL_collection_eff, mod_EOL_collected_recycled, mod_Repowering, mod_Repairing, mod_reliability_t50, mod_reliability_t90, mod_lifetime</t>
-  </si>
-  <si>
     <t>AbsRel</t>
   </si>
   <si>
@@ -157,6 +145,18 @@
   </si>
   <si>
     <t>mat_MFG_scrap_Recycled_into_HQ</t>
+  </si>
+  <si>
+    <t>mod_Repair</t>
+  </si>
+  <si>
+    <t>mod_Reuse</t>
+  </si>
+  <si>
+    <t>mod_EOL_collection_eff, mod_EOL_collected_recycled, mod_Repair, mod_Reuse</t>
+  </si>
+  <si>
+    <t>mod_EOL_collection_eff, mod_EOL_collected_recycled, mod_Repair, mod_Reuse, mod_reliability_t50, mod_reliability_t90, mod_lifetime</t>
   </si>
 </sst>
 </file>
@@ -510,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1843FE10-D458-44C9-982C-7968BE305E92}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D17" sqref="C17:D17"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,10 +524,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -536,13 +536,13 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -565,7 +565,7 @@
         <v>-10</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -588,7 +588,7 @@
         <v>-10</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -611,7 +611,7 @@
         <v>-10</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -634,7 +634,7 @@
         <v>-10</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -657,7 +657,7 @@
         <v>-10</v>
       </c>
       <c r="G6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -668,10 +668,10 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E7">
         <v>10</v>
@@ -680,7 +680,7 @@
         <v>-10</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -703,7 +703,7 @@
         <v>-10</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -717,7 +717,7 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -726,7 +726,7 @@
         <v>-10</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -749,7 +749,7 @@
         <v>-10</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -772,7 +772,7 @@
         <v>-10</v>
       </c>
       <c r="G11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -795,7 +795,7 @@
         <v>-10</v>
       </c>
       <c r="G12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -818,7 +818,7 @@
         <v>-10</v>
       </c>
       <c r="G13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -832,7 +832,7 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E14">
         <v>10</v>
@@ -841,7 +841,7 @@
         <v>-10</v>
       </c>
       <c r="G14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -864,7 +864,7 @@
         <v>-10</v>
       </c>
       <c r="G15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -887,7 +887,7 @@
         <v>-10</v>
       </c>
       <c r="G16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -901,7 +901,7 @@
         <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E17">
         <v>10</v>
@@ -910,7 +910,7 @@
         <v>-10</v>
       </c>
       <c r="G17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -933,7 +933,7 @@
         <v>-10</v>
       </c>
       <c r="G18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -956,7 +956,7 @@
         <v>-10</v>
       </c>
       <c r="G19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -979,7 +979,7 @@
         <v>-10</v>
       </c>
       <c r="G20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -990,10 +990,10 @@
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="E21">
         <v>10</v>
@@ -1002,7 +1002,7 @@
         <v>-10</v>
       </c>
       <c r="G21" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1013,10 +1013,10 @@
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E22">
         <v>10</v>
@@ -1025,7 +1025,7 @@
         <v>-10</v>
       </c>
       <c r="G22" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1036,10 +1036,10 @@
         <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E23">
         <v>10</v>
@@ -1048,7 +1048,7 @@
         <v>-10</v>
       </c>
       <c r="G23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1059,10 +1059,10 @@
         <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E24">
         <v>10</v>
@@ -1071,7 +1071,7 @@
         <v>-10</v>
       </c>
       <c r="G24" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>